<commit_message>
Updated data provider excel
</commit_message>
<xml_diff>
--- a/spreads/data.xlsx
+++ b/spreads/data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22821"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4485C7B1-5074-4D62-9ADE-3A58D58FEAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{134CDA88-EC58-4825-BE1E-58F92ED1924F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="another" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -49,6 +50,24 @@
   </si>
   <si>
     <t>user03</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test22</t>
+  </si>
+  <si>
+    <t>test33</t>
   </si>
 </sst>
 </file>
@@ -402,7 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +462,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFA7192-6041-4BB0-AE9F-DE6B7A78D143}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>